<commit_message>
update sprints.xlsx requirement.xlsx and eweather_Gantt.mpp
</commit_message>
<xml_diff>
--- a/documents/requirement.xlsx
+++ b/documents/requirement.xlsx
@@ -4,21 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="75" windowWidth="20100" windowHeight="8235" activeTab="4"/>
+    <workbookView xWindow="195" yWindow="75" windowWidth="20100" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="req list" sheetId="1" r:id="rId1"/>
     <sheet name="sprints" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Φύλλο1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="89">
   <si>
     <t>Χρήση openweathermap API και JSON API για την ενημέρωση των τρεχουσών καιρικών δεδομένων.</t>
   </si>
@@ -318,34 +315,6 @@
     <t>Σύνολο ωρών</t>
   </si>
   <si>
-    <r>
-      <t>Πρόβλεψη καιρού 1</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ης</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ημέρας (αντίστοιχο κουμπί).</t>
-    </r>
-  </si>
-  <si>
     <t>5.2</t>
   </si>
   <si>
@@ -365,7 +334,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,45 +441,6 @@
       <family val="2"/>
       <charset val="161"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="161"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="161"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="161"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="161"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -670,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -746,41 +676,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -798,17 +693,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1221,7 +1105,7 @@
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="4"/>
       <c r="B6" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>3</v>
@@ -1798,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:E46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1808,8 +1692,8 @@
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="16" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="41.45" customHeight="1" thickBot="1">
@@ -1827,12 +1711,12 @@
       </c>
     </row>
     <row r="2" spans="2:5" ht="22.9" customHeight="1" thickBot="1">
-      <c r="B2" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:5" ht="15.75">
       <c r="B3" s="13">
@@ -1892,7 +1776,7 @@
     </row>
     <row r="7" spans="2:5" ht="30.75">
       <c r="B7" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>3</v>
@@ -2080,12 +1964,12 @@
       </c>
     </row>
     <row r="22" spans="2:5" ht="22.15" customHeight="1" thickBot="1">
-      <c r="B22" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
+      <c r="B22" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
     </row>
     <row r="23" spans="2:5" ht="15.75">
       <c r="B23" s="13" t="s">
@@ -2179,7 +2063,7 @@
     </row>
     <row r="30" spans="2:5" ht="30.75">
       <c r="B30" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>14</v>
@@ -2257,12 +2141,12 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B36" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
+      <c r="B36" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
     </row>
     <row r="37" spans="2:5" ht="15.75">
       <c r="B37" s="13" t="s">
@@ -2400,1013 +2284,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="51" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" style="36" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="51" customHeight="1" thickBot="1">
-      <c r="A1" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A2" s="40">
-        <v>1</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="27.75" customHeight="1">
-      <c r="A3" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="38.25" customHeight="1">
-      <c r="A4" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="42">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A5" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="A6" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="23.25" customHeight="1">
-      <c r="A7" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="21.75" customHeight="1">
-      <c r="A8" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="21.75" customHeight="1">
-      <c r="A9" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="42">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A10" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="32.25" customHeight="1">
-      <c r="A11" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" customHeight="1">
-      <c r="A12" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" customHeight="1">
-      <c r="A13" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="21.75" customHeight="1">
-      <c r="A14" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18" customHeight="1">
-      <c r="A15" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="29.25" customHeight="1">
-      <c r="A16" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30.75" customHeight="1">
-      <c r="A17" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="24.75" customHeight="1">
-      <c r="A18" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="22.5" customHeight="1">
-      <c r="A19" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="31.5" customHeight="1">
-      <c r="A20" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="23.25" customHeight="1">
-      <c r="A21" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A22" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="21" customHeight="1">
-      <c r="A23" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="29.25" customHeight="1">
-      <c r="A24" s="40">
-        <v>5.2</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1">
-      <c r="A25" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A26" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="21.75" customHeight="1">
-      <c r="A27" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="23.25" customHeight="1">
-      <c r="A28" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="24" customHeight="1">
-      <c r="A29" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A30" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="29.25" customHeight="1">
-      <c r="A31" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A32" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A33" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A34" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="23.25" customHeight="1">
-      <c r="A35" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="21.75" customHeight="1">
-      <c r="A36" s="44">
-        <v>8</v>
-      </c>
-      <c r="B36" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="42">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C36"/>
-  <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection sqref="A1:C36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="42.140625" defaultRowHeight="28.5" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="47" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" style="42" customWidth="1"/>
-    <col min="3" max="3" width="15" style="42" customWidth="1"/>
-    <col min="4" max="16384" width="42.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A1" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A2" s="40">
-        <v>1</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A3" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A4" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A6" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" customHeight="1">
-      <c r="A7" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A8" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A9" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A10" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A11" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A12" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A13" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A14" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18" customHeight="1">
-      <c r="A15" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A16" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A17" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A18" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="12.75">
-      <c r="A19" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A20" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A21" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A22" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A23" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A24" s="40">
-        <v>5.2</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="21" customHeight="1">
-      <c r="A25" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A26" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="27" customHeight="1">
-      <c r="A27" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A28" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18" customHeight="1">
-      <c r="A29" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A30" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A31" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A32" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18" customHeight="1">
-      <c r="A33" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="18" customHeight="1">
-      <c r="A34" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A35" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="18" customHeight="1">
-      <c r="A36" s="44">
-        <v>8</v>
-      </c>
-      <c r="B36" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="42">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="A1:D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="24" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="8" style="56" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" style="57" customWidth="1"/>
-    <col min="3" max="16384" width="12.5703125" style="56"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="24" customHeight="1" thickBot="1">
-      <c r="A1" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="55" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="24" customHeight="1" thickBot="1">
-      <c r="A2" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-    </row>
-    <row r="3" spans="1:4" ht="24" customHeight="1">
-      <c r="A3" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="15">
-        <v>4</v>
-      </c>
-      <c r="D3" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="24" customHeight="1">
-      <c r="A4" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="19">
-        <v>4</v>
-      </c>
-      <c r="D4" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="24" customHeight="1">
-      <c r="A5" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="19">
-        <v>4</v>
-      </c>
-      <c r="D5" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="24" customHeight="1">
-      <c r="A6" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="19">
-        <v>4</v>
-      </c>
-      <c r="D6" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="24" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:4" ht="24" customHeight="1">
-      <c r="A8" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="19">
-        <v>4</v>
-      </c>
-      <c r="D8" s="20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="24" customHeight="1">
-      <c r="A9" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="19">
-        <v>4</v>
-      </c>
-      <c r="D9" s="20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="24" customHeight="1">
-      <c r="A10" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="19">
-        <v>4</v>
-      </c>
-      <c r="D10" s="20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1" thickBot="1">
-      <c r="A11" s="28">
-        <v>8</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="24">
-        <v>4</v>
-      </c>
-      <c r="D11" s="25">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="24" customHeight="1" thickBot="1">
-      <c r="A12"/>
-      <c r="B12" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="26">
-        <f>SUM(C3:C11)</f>
-        <v>32</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:D2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>